<commit_message>
Minor update to perf spreadsheet.
</commit_message>
<xml_diff>
--- a/perf/rtt.xlsx
+++ b/perf/rtt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ouster\Documents\code\homaModule\perf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF25095A-86C0-4FC6-96A7-7EB57D472263}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4B7780-BC34-487C-8966-E2F4A680B0E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14610" yWindow="1410" windowWidth="19095" windowHeight="15435" xr2:uid="{F862E3F9-BE5F-4B69-B28A-458A49A62563}"/>
+    <workbookView xWindow="22680" yWindow="1575" windowWidth="19095" windowHeight="15435" xr2:uid="{F862E3F9-BE5F-4B69-B28A-458A49A62563}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>